<commit_message>
refactoring - refactoring Elo formula. Now it's work correctly.
</commit_message>
<xml_diff>
--- a/2Расстановки.xlsx
+++ b/2Расстановки.xlsx
@@ -12540,8 +12540,8 @@
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.5546875" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -14045,7 +14045,7 @@
   <dimension ref="A1:L32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.5546875" defaultRowHeight="18" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
refactoring - create_temp_players (add new attribute self-players and change all code to use it) in fitire it will have make code more optimal
</commit_message>
<xml_diff>
--- a/2Расстановки.xlsx
+++ b/2Расстановки.xlsx
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1208" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1208" uniqueCount="30">
   <si>
     <t>Левая площадка</t>
   </si>
@@ -164,18 +164,6 @@
   </si>
   <si>
     <t>Ксения</t>
-  </si>
-  <si>
-    <t>Петя</t>
-  </si>
-  <si>
-    <t>Петя1</t>
-  </si>
-  <si>
-    <t>Петя2</t>
-  </si>
-  <si>
-    <t>Петя3</t>
   </si>
 </sst>
 </file>
@@ -1021,8 +1009,8 @@
   </sheetPr>
   <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19:E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.5546875" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -1076,16 +1064,16 @@
         <v>1</v>
       </c>
       <c r="B3" s="32" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="C3" s="33" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="D3" s="34" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="E3" s="35" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="F3" s="36">
         <f>$B$1</f>
@@ -1111,16 +1099,16 @@
         <v>2</v>
       </c>
       <c r="B5" s="32" t="s">
-        <v>30</v>
-      </c>
-      <c r="C5" s="34" t="s">
-        <v>31</v>
+        <v>14</v>
+      </c>
+      <c r="C5" s="33" t="s">
+        <v>20</v>
       </c>
       <c r="D5" s="34" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="E5" s="35" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="F5" s="36">
         <f>$F$1</f>
@@ -1146,16 +1134,16 @@
         <v>3</v>
       </c>
       <c r="B7" s="32" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="C7" s="33" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="D7" s="34" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="E7" s="35" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="F7" s="36">
         <f>$E$1</f>
@@ -1181,16 +1169,16 @@
         <v>4</v>
       </c>
       <c r="B9" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="33" t="s">
-        <v>5</v>
-      </c>
       <c r="D9" s="34" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="E9" s="35" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="F9" s="36">
         <f>$C$1</f>
@@ -1216,16 +1204,16 @@
         <v>5</v>
       </c>
       <c r="B11" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="33" t="s">
-        <v>5</v>
-      </c>
       <c r="D11" s="34" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="E11" s="35" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="F11" s="36">
         <f>$D$1</f>
@@ -1251,16 +1239,16 @@
         <v>6</v>
       </c>
       <c r="B13" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="33" t="s">
-        <v>5</v>
-      </c>
       <c r="D13" s="34" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="E13" s="35" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="F13" s="36">
         <f>$B$1</f>
@@ -1286,16 +1274,16 @@
         <v>7</v>
       </c>
       <c r="B15" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="33" t="s">
-        <v>5</v>
-      </c>
       <c r="D15" s="34" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="E15" s="35" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="F15" s="36">
         <f>$F$1</f>
@@ -1321,16 +1309,16 @@
         <v>8</v>
       </c>
       <c r="B17" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="33" t="s">
-        <v>5</v>
-      </c>
       <c r="D17" s="34" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="E17" s="35" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="F17" s="36">
         <f>$E$1</f>
@@ -1356,16 +1344,16 @@
         <v>9</v>
       </c>
       <c r="B19" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="33" t="s">
-        <v>5</v>
-      </c>
       <c r="D19" s="34" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="F19" s="36">
         <f>$C$1</f>
@@ -1585,6 +1573,11 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="A31:A32"/>
     <mergeCell ref="A21:A22"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="D2:E2"/>
@@ -1597,11 +1590,6 @@
     <mergeCell ref="A15:A16"/>
     <mergeCell ref="A17:A18"/>
     <mergeCell ref="A19:A20"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="A31:A32"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="85" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -2431,6 +2419,13 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="A29:A30"/>
     <mergeCell ref="A17:A18"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="D2:E2"/>
@@ -2443,13 +2438,6 @@
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="A13:A14"/>
     <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="A29:A30"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="70" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -3134,12 +3122,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="A5:A6"/>
     <mergeCell ref="A31:A32"/>
     <mergeCell ref="A9:A10"/>
     <mergeCell ref="A11:A12"/>
@@ -3152,6 +3134,12 @@
     <mergeCell ref="A25:A26"/>
     <mergeCell ref="A27:A28"/>
     <mergeCell ref="A29:A30"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A5:A6"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="85" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -3745,11 +3733,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="A7:A8"/>
     <mergeCell ref="A31:A32"/>
     <mergeCell ref="A9:A10"/>
     <mergeCell ref="A11:A12"/>
@@ -3762,6 +3745,11 @@
     <mergeCell ref="A25:A26"/>
     <mergeCell ref="A27:A28"/>
     <mergeCell ref="A29:A30"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="A7:A8"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="85" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -4486,14 +4474,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="A9:A10"/>
     <mergeCell ref="A25:A26"/>
     <mergeCell ref="A27:A28"/>
     <mergeCell ref="A29:A30"/>
@@ -4504,6 +4484,14 @@
     <mergeCell ref="A19:A20"/>
     <mergeCell ref="A21:A22"/>
     <mergeCell ref="A23:A24"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A9:A10"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="85" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -5248,6 +5236,8 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A5:A6"/>
     <mergeCell ref="A31:A32"/>
     <mergeCell ref="A27:A28"/>
     <mergeCell ref="A29:A30"/>
@@ -5264,8 +5254,6 @@
     <mergeCell ref="A17:A18"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="D2:E2"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="A5:A6"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="53" orientation="landscape" verticalDpi="0" r:id="rId1"/>
@@ -6099,6 +6087,13 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="A29:A30"/>
     <mergeCell ref="A17:A18"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="D2:E2"/>
@@ -6111,13 +6106,6 @@
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="A13:A14"/>
     <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="A29:A30"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="70" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -7025,6 +7013,14 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="A27:A28"/>
     <mergeCell ref="A15:A16"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="D2:E2"/>
@@ -7036,14 +7032,6 @@
     <mergeCell ref="A9:A10"/>
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="A13:A14"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="A27:A28"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="63" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -8030,6 +8018,14 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="A27:A28"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="A15:A16"/>
@@ -8042,14 +8038,6 @@
     <mergeCell ref="A9:A10"/>
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="A13:A14"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="A27:A28"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="57" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -9115,11 +9103,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="A25:A26"/>
     <mergeCell ref="J2:L2"/>
     <mergeCell ref="A15:A16"/>
     <mergeCell ref="A17:A18"/>
@@ -9135,6 +9118,11 @@
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="H2:I2"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="A25:A26"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="53" orientation="landscape" verticalDpi="0" r:id="rId1"/>
@@ -10281,6 +10269,15 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="A25:A26"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="L2:M2"/>
     <mergeCell ref="A13:A14"/>
@@ -10293,15 +10290,6 @@
     <mergeCell ref="A7:A8"/>
     <mergeCell ref="A9:A10"/>
     <mergeCell ref="A11:A12"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="A25:A26"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="53" orientation="landscape" verticalDpi="0" r:id="rId1"/>
@@ -11127,13 +11115,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="A29:A30"/>
     <mergeCell ref="A17:A18"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="D2:E2"/>
@@ -11146,6 +11127,13 @@
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="A13:A14"/>
     <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="A29:A30"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="70" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -12374,17 +12362,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="A11:A12"/>
     <mergeCell ref="A25:A26"/>
     <mergeCell ref="A27:A28"/>
     <mergeCell ref="A29:A30"/>
@@ -12395,6 +12372,17 @@
     <mergeCell ref="A19:A20"/>
     <mergeCell ref="A21:A22"/>
     <mergeCell ref="A23:A24"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:K2"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="53" orientation="landscape" verticalDpi="0" r:id="rId1"/>
@@ -13702,18 +13690,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="N2:O2"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="L2:M2"/>
     <mergeCell ref="A25:A26"/>
     <mergeCell ref="A27:A28"/>
     <mergeCell ref="A29:A30"/>
@@ -13724,6 +13700,18 @@
     <mergeCell ref="A19:A20"/>
     <mergeCell ref="A21:A22"/>
     <mergeCell ref="A23:A24"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="53" orientation="landscape" verticalDpi="0" r:id="rId1"/>
@@ -15110,16 +15098,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="N2:P2"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="L2:M2"/>
     <mergeCell ref="A31:A32"/>
     <mergeCell ref="A9:A10"/>
     <mergeCell ref="A11:A12"/>
@@ -15132,6 +15110,16 @@
     <mergeCell ref="A25:A26"/>
     <mergeCell ref="A27:A28"/>
     <mergeCell ref="A29:A30"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="N2:P2"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="L2:M2"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="53" orientation="landscape" verticalDpi="0" r:id="rId1"/>
@@ -16599,6 +16587,21 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="P2:Q2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="L2:M2"/>
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="A13:A14"/>
     <mergeCell ref="A15:A16"/>
@@ -16607,21 +16610,6 @@
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="A7:A8"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="N2:O2"/>
-    <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="A21:A22"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="51" orientation="landscape" verticalDpi="0" r:id="rId1"/>
@@ -18171,17 +18159,6 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="N2:O2"/>
-    <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="L2:M2"/>
     <mergeCell ref="A31:A32"/>
     <mergeCell ref="A9:A10"/>
     <mergeCell ref="A11:A12"/>
@@ -18194,6 +18171,17 @@
     <mergeCell ref="A25:A26"/>
     <mergeCell ref="A27:A28"/>
     <mergeCell ref="A29:A30"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="P2:Q2"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="L2:M2"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="48" orientation="landscape" verticalDpi="0" r:id="rId1"/>
@@ -19827,14 +19815,6 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="A23:A24"/>
     <mergeCell ref="R2:S2"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="H2:I2"/>
@@ -19851,6 +19831,14 @@
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="A7:A8"/>
     <mergeCell ref="A9:A10"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="A23:A24"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="46" orientation="landscape" verticalDpi="0" r:id="rId1"/>
@@ -21558,15 +21546,6 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="R2:T2"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="N2:O2"/>
-    <mergeCell ref="P2:Q2"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="A7:A8"/>
@@ -21582,6 +21561,15 @@
     <mergeCell ref="A25:A26"/>
     <mergeCell ref="A27:A28"/>
     <mergeCell ref="A29:A30"/>
+    <mergeCell ref="R2:T2"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="P2:Q2"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="43" orientation="landscape" verticalDpi="0" r:id="rId1"/>
@@ -23370,15 +23358,6 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="A19:A20"/>
     <mergeCell ref="T2:U2"/>
     <mergeCell ref="A21:A22"/>
     <mergeCell ref="A23:A24"/>
@@ -23395,6 +23374,15 @@
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="H2:I2"/>
     <mergeCell ref="J2:K2"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="A19:A20"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="41" orientation="landscape" verticalDpi="0" r:id="rId1"/>
@@ -23988,6 +23976,11 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="A31:A32"/>
     <mergeCell ref="A21:A22"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="D2:E2"/>
@@ -24000,11 +23993,6 @@
     <mergeCell ref="A15:A16"/>
     <mergeCell ref="A17:A18"/>
     <mergeCell ref="A19:A20"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="A31:A32"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="85" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -24831,6 +24819,13 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="A29:A30"/>
     <mergeCell ref="A17:A18"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="D2:E2"/>
@@ -24843,13 +24838,6 @@
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="A13:A14"/>
     <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="A29:A30"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="70" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -25996,6 +25984,15 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="A25:A26"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="L2:M2"/>
     <mergeCell ref="A13:A14"/>
@@ -26008,15 +26005,6 @@
     <mergeCell ref="A7:A8"/>
     <mergeCell ref="A9:A10"/>
     <mergeCell ref="A11:A12"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="A25:A26"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="53" orientation="landscape" verticalDpi="0" r:id="rId1"/>
@@ -26843,6 +26831,13 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="A29:A30"/>
     <mergeCell ref="A17:A18"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="D2:E2"/>
@@ -26855,13 +26850,6 @@
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="A13:A14"/>
     <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="A29:A30"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="70" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -28008,6 +27996,15 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="A25:A26"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="L2:M2"/>
     <mergeCell ref="A13:A14"/>
@@ -28020,15 +28017,6 @@
     <mergeCell ref="A7:A8"/>
     <mergeCell ref="A9:A10"/>
     <mergeCell ref="A11:A12"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="A25:A26"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="53" orientation="landscape" verticalDpi="0" r:id="rId1"/>
@@ -29496,6 +29484,21 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="P2:Q2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="L2:M2"/>
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="A13:A14"/>
     <mergeCell ref="A15:A16"/>
@@ -29504,21 +29507,6 @@
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="A7:A8"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="N2:O2"/>
-    <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="A21:A22"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="51" orientation="landscape" verticalDpi="0" r:id="rId1"/>
@@ -30346,6 +30334,13 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="A29:A30"/>
     <mergeCell ref="A17:A18"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="D2:E2"/>
@@ -30358,13 +30353,6 @@
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="A13:A14"/>
     <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="A29:A30"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="70" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>